<commit_message>
Excel Finish, but with trash
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -3,20 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
-  <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
-  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Лист1" state="visible" r:id="rId4"/>
-    <sheet sheetId="2" name="Лист2" state="visible" r:id="rId5"/>
-    <sheet sheetId="3" name="Лист3" state="visible" r:id="rId6"/>
+    <sheet sheetId="1" name="Data" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="20">
   <si>
     <t>label</t>
   </si>
@@ -27,6 +22,12 @@
     <t>data</t>
   </si>
   <si>
+    <t>Об`єм (маса) каналу витрати 1</t>
+  </si>
+  <si>
+    <t>10:10:2020:0</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
@@ -45,9 +46,6 @@
     <t>Значення температури ТСП 1 * 100</t>
   </si>
   <si>
-    <t>10:10:2020:0</t>
-  </si>
-  <si>
     <t>Значення температури ТСП 2 * 100</t>
   </si>
   <si>
@@ -69,7 +67,7 @@
     <t>Температура всередині корпусу</t>
   </si>
   <si>
-    <t>Об`єм (маса) каналу витрати 1</t>
+    <t/>
   </si>
   <si>
     <t/>
@@ -276,20 +274,16 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
+                <a:tint val="100000"/>
+                <a:shade val="100000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
+                <a:tint val="50000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -411,18 +405,54 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </a:style>
+    </a:spDef>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C81"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0"/>
+  <dimension ref="A1:C61"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="64" style="1" customWidth="1"/>
     <col min="2" max="2" width="32" customWidth="1"/>
@@ -445,18 +475,18 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -464,10 +494,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -475,10 +505,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -486,10 +516,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -497,10 +527,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C9">
         <v>22.72</v>
@@ -508,10 +538,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C10">
         <v>22.1</v>
@@ -519,10 +549,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C11">
         <v>21.85</v>
@@ -530,10 +560,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C12">
         <v>21.68</v>
@@ -541,10 +571,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C13">
         <v>21.73</v>
@@ -552,10 +582,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C15">
         <v>22.73</v>
@@ -563,10 +593,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C16">
         <v>22.13</v>
@@ -574,10 +604,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B17" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C17">
         <v>21.84</v>
@@ -585,10 +615,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C18">
         <v>21.73</v>
@@ -596,10 +626,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C19">
         <v>21.77</v>
@@ -607,10 +637,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B21" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -618,10 +648,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -629,10 +659,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B23" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -640,10 +670,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B24" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -651,10 +681,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -662,10 +692,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B27" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C27">
         <v>9.13861111111111</v>
@@ -673,10 +703,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B28" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C28">
         <v>9.13861111111111</v>
@@ -684,10 +714,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B29" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C29">
         <v>9.13861111111111</v>
@@ -695,10 +725,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B30" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C30">
         <v>9.13861111111111</v>
@@ -706,10 +736,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B31" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C31">
         <v>9.13861111111111</v>
@@ -717,10 +747,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B33" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C33">
         <v>9.13861111111111</v>
@@ -728,10 +758,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B34" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C34">
         <v>9.13861111111111</v>
@@ -739,10 +769,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B35" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C35">
         <v>9.13861111111111</v>
@@ -750,10 +780,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B36" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C36">
         <v>9.13861111111111</v>
@@ -761,10 +791,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B37" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C37">
         <v>9.0675</v>
@@ -772,10 +802,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B39" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C39">
         <v>0.5</v>
@@ -783,10 +813,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B40" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C40">
         <v>0.5</v>
@@ -794,10 +824,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B41" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C41">
         <v>0.5</v>
@@ -805,10 +835,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B42" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C42">
         <v>0.5</v>
@@ -816,10 +846,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B43" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C43">
         <v>0.5</v>
@@ -827,10 +857,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B45" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C45">
         <v>0.4</v>
@@ -838,10 +868,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B46" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C46">
         <v>0.4</v>
@@ -849,10 +879,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B47" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C47">
         <v>0.4</v>
@@ -860,10 +890,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B48" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C48">
         <v>0.4</v>
@@ -871,10 +901,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B49" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C49">
         <v>0.4</v>
@@ -882,10 +912,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B51" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C51">
         <v>8833</v>
@@ -893,10 +923,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B52" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C52">
         <v>8833</v>
@@ -904,10 +934,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B53" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C53">
         <v>8833</v>
@@ -915,10 +945,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B54" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C54">
         <v>8577</v>
@@ -926,10 +956,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B55" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C55">
         <v>1921</v>
@@ -937,194 +967,61 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B57" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C57" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B58" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C58" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B59" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C59" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B60" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C60" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B61" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C61" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B63" t="s">
-        <v>9</v>
-      </c>
-      <c r="C63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B65" t="s">
-        <v>9</v>
-      </c>
-      <c r="C65">
-        <v>22.72</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B67" t="s">
-        <v>9</v>
-      </c>
-      <c r="C67">
-        <v>22.73</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B69" t="s">
-        <v>9</v>
-      </c>
-      <c r="C69">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B71" t="s">
-        <v>9</v>
-      </c>
-      <c r="C71">
-        <v>9.13861111111111</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B73" t="s">
-        <v>9</v>
-      </c>
-      <c r="C73">
-        <v>9.13861111111111</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B75" t="s">
-        <v>9</v>
-      </c>
-      <c r="C75">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B77" t="s">
-        <v>9</v>
-      </c>
-      <c r="C77">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B79" t="s">
-        <v>9</v>
-      </c>
-      <c r="C79">
-        <v>8833</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B81" t="s">
-        <v>9</v>
-      </c>
-      <c r="C81" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
download Excel and send to mail
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="40">
   <si>
     <t>label</t>
   </si>
@@ -25,22 +25,79 @@
     <t>Об`єм (маса) каналу витрати 1</t>
   </si>
   <si>
-    <t>10:10:2020:0</t>
+    <t>12:10:2020:1</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>11:10:2020:0</t>
-  </si>
-  <si>
-    <t>12:10:2020:0</t>
-  </si>
-  <si>
-    <t>13:10:2020:0</t>
-  </si>
-  <si>
-    <t>14:10:2020:0</t>
+    <t>13:10:2020:1</t>
+  </si>
+  <si>
+    <t>14:10:2020:1</t>
+  </si>
+  <si>
+    <t>15:10:2020:1</t>
+  </si>
+  <si>
+    <t>16:10:2020:1</t>
+  </si>
+  <si>
+    <t>17:10:2020:1</t>
+  </si>
+  <si>
+    <t>18:10:2020:1</t>
+  </si>
+  <si>
+    <t>19:10:2020:1</t>
+  </si>
+  <si>
+    <t>20:10:2020:1</t>
+  </si>
+  <si>
+    <t>21:10:2020:1</t>
+  </si>
+  <si>
+    <t>22:10:2020:1</t>
+  </si>
+  <si>
+    <t>23:10:2020:1</t>
+  </si>
+  <si>
+    <t>24:10:2020:1</t>
+  </si>
+  <si>
+    <t>25:10:2020:1</t>
+  </si>
+  <si>
+    <t>26:10:2020:1</t>
+  </si>
+  <si>
+    <t>27:10:2020:1</t>
+  </si>
+  <si>
+    <t>28:10:2020:1</t>
+  </si>
+  <si>
+    <t>29:10:2020:1</t>
+  </si>
+  <si>
+    <t>30:10:2020:1</t>
+  </si>
+  <si>
+    <t>1:11:2020:1</t>
+  </si>
+  <si>
+    <t>2:11:2020:1</t>
+  </si>
+  <si>
+    <t>3:11:2020:1</t>
+  </si>
+  <si>
+    <t>4:11:2020:1</t>
+  </si>
+  <si>
+    <t>5:11:2020:1</t>
   </si>
   <si>
     <t>Значення температури ТСП 1 * 100</t>
@@ -65,6 +122,9 @@
   </si>
   <si>
     <t>Температура всередині корпусу</t>
+  </si>
+  <si>
+    <t/>
   </si>
   <si>
     <t/>
@@ -451,7 +511,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C61"/>
+  <dimension ref="A1:C251"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="64" style="1" customWidth="1"/>
@@ -525,15 +585,26 @@
         <v>0</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+    </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C9">
-        <v>22.72</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -541,10 +612,10 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C10">
-        <v>22.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -552,10 +623,10 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C11">
-        <v>21.85</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -563,10 +634,10 @@
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C12">
-        <v>21.68</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -574,21 +645,32 @@
         <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C13">
-        <v>21.73</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C15">
-        <v>22.73</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -596,10 +678,10 @@
         <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C16">
-        <v>22.13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -607,10 +689,10 @@
         <v>5</v>
       </c>
       <c r="B17" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C17">
-        <v>21.84</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -618,10 +700,10 @@
         <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C18">
-        <v>21.73</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -629,18 +711,29 @@
         <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C19">
-        <v>21.77</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B21" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -651,7 +744,7 @@
         <v>5</v>
       </c>
       <c r="B22" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -662,7 +755,7 @@
         <v>5</v>
       </c>
       <c r="B23" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -673,7 +766,7 @@
         <v>5</v>
       </c>
       <c r="B24" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -684,32 +777,32 @@
         <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="C25">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B27" t="s">
-        <v>4</v>
-      </c>
-      <c r="C27">
-        <v>9.13861111111111</v>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C28">
-        <v>9.13861111111111</v>
+        <v>21.85</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -717,10 +810,10 @@
         <v>5</v>
       </c>
       <c r="B29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C29">
-        <v>9.13861111111111</v>
+        <v>21.68</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -728,10 +821,10 @@
         <v>5</v>
       </c>
       <c r="B30" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C30">
-        <v>9.13861111111111</v>
+        <v>21.73</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -739,21 +832,32 @@
         <v>5</v>
       </c>
       <c r="B31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31">
+        <v>21.74</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" t="s">
         <v>9</v>
       </c>
-      <c r="C31">
-        <v>9.13861111111111</v>
+      <c r="C32">
+        <v>21.4</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B33" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C33">
-        <v>9.13861111111111</v>
+        <v>20.85</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -761,10 +865,10 @@
         <v>5</v>
       </c>
       <c r="B34" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C34">
-        <v>9.13861111111111</v>
+        <v>20.84</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -772,10 +876,10 @@
         <v>5</v>
       </c>
       <c r="B35" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C35">
-        <v>9.13861111111111</v>
+        <v>20.81</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -783,10 +887,10 @@
         <v>5</v>
       </c>
       <c r="B36" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C36">
-        <v>9.13861111111111</v>
+        <v>20.74</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -794,21 +898,32 @@
         <v>5</v>
       </c>
       <c r="B37" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C37">
-        <v>9.0675</v>
+        <v>20.79</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B38" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38">
+        <v>20.67</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B39" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C39">
-        <v>0.5</v>
+        <v>20.81</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -816,10 +931,10 @@
         <v>5</v>
       </c>
       <c r="B40" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C40">
-        <v>0.5</v>
+        <v>21.03</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -827,10 +942,10 @@
         <v>5</v>
       </c>
       <c r="B41" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C41">
-        <v>0.5</v>
+        <v>21.35</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -838,10 +953,10 @@
         <v>5</v>
       </c>
       <c r="B42" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="C42">
-        <v>0.5</v>
+        <v>21.66</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -849,21 +964,32 @@
         <v>5</v>
       </c>
       <c r="B43" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C43">
-        <v>0.5</v>
+        <v>21.63</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B44" t="s">
+        <v>21</v>
+      </c>
+      <c r="C44">
+        <v>21.57</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B45" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="C45">
-        <v>0.4</v>
+        <v>21.27</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -871,10 +997,10 @@
         <v>5</v>
       </c>
       <c r="B46" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C46">
-        <v>0.4</v>
+        <v>21.13</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -882,10 +1008,10 @@
         <v>5</v>
       </c>
       <c r="B47" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C47">
-        <v>0.4</v>
+        <v>20.99</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -893,10 +1019,10 @@
         <v>5</v>
       </c>
       <c r="B48" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="C48">
-        <v>0.4</v>
+        <v>20.92</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -904,43 +1030,43 @@
         <v>5</v>
       </c>
       <c r="B49" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="C49">
-        <v>0.4</v>
+        <v>20.77</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B50" t="s">
+        <v>27</v>
+      </c>
+      <c r="C50">
+        <v>20.26</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B51" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="C51">
-        <v>8833</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B52" t="s">
-        <v>6</v>
-      </c>
-      <c r="C52">
-        <v>8833</v>
+        <v>19.79</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="B53" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C53">
-        <v>8833</v>
+        <v>21.84</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -948,10 +1074,10 @@
         <v>5</v>
       </c>
       <c r="B54" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C54">
-        <v>8577</v>
+        <v>21.73</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -959,21 +1085,32 @@
         <v>5</v>
       </c>
       <c r="B55" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C55">
-        <v>1921</v>
+        <v>21.77</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B56" t="s">
+        <v>8</v>
+      </c>
+      <c r="C56">
+        <v>21.78</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B57" t="s">
-        <v>4</v>
-      </c>
-      <c r="C57" t="s">
-        <v>18</v>
+        <v>9</v>
+      </c>
+      <c r="C57">
+        <v>21.42</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -981,10 +1118,10 @@
         <v>5</v>
       </c>
       <c r="B58" t="s">
-        <v>6</v>
-      </c>
-      <c r="C58" t="s">
-        <v>19</v>
+        <v>10</v>
+      </c>
+      <c r="C58">
+        <v>20.88</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -992,10 +1129,10 @@
         <v>5</v>
       </c>
       <c r="B59" t="s">
-        <v>7</v>
-      </c>
-      <c r="C59" t="s">
-        <v>19</v>
+        <v>11</v>
+      </c>
+      <c r="C59">
+        <v>20.87</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -1003,10 +1140,10 @@
         <v>5</v>
       </c>
       <c r="B60" t="s">
-        <v>8</v>
-      </c>
-      <c r="C60" t="s">
-        <v>19</v>
+        <v>12</v>
+      </c>
+      <c r="C60">
+        <v>20.81</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -1014,10 +1151,2023 @@
         <v>5</v>
       </c>
       <c r="B61" t="s">
+        <v>13</v>
+      </c>
+      <c r="C61">
+        <v>20.77</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B62" t="s">
+        <v>14</v>
+      </c>
+      <c r="C62">
+        <v>20.82</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B63" t="s">
+        <v>15</v>
+      </c>
+      <c r="C63">
+        <v>20.68</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B64" t="s">
+        <v>16</v>
+      </c>
+      <c r="C64">
+        <v>20.83</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B65" t="s">
+        <v>17</v>
+      </c>
+      <c r="C65">
+        <v>21.05</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B66" t="s">
+        <v>18</v>
+      </c>
+      <c r="C66">
+        <v>21.39</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B67" t="s">
+        <v>19</v>
+      </c>
+      <c r="C67">
+        <v>21.68</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B68" t="s">
+        <v>20</v>
+      </c>
+      <c r="C68">
+        <v>21.66</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B69" t="s">
+        <v>21</v>
+      </c>
+      <c r="C69">
+        <v>21.6</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B70" t="s">
+        <v>22</v>
+      </c>
+      <c r="C70">
+        <v>21.3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B71" t="s">
+        <v>23</v>
+      </c>
+      <c r="C71">
+        <v>21.15</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B72" t="s">
+        <v>24</v>
+      </c>
+      <c r="C72">
+        <v>21.01</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B73" t="s">
+        <v>25</v>
+      </c>
+      <c r="C73">
+        <v>20.95</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B74" t="s">
+        <v>26</v>
+      </c>
+      <c r="C74">
+        <v>20.79</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B75" t="s">
+        <v>27</v>
+      </c>
+      <c r="C75">
+        <v>20.27</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B76" t="s">
+        <v>28</v>
+      </c>
+      <c r="C76">
+        <v>19.82</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B78" t="s">
+        <v>4</v>
+      </c>
+      <c r="C78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B79" t="s">
+        <v>6</v>
+      </c>
+      <c r="C79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B80" t="s">
+        <v>7</v>
+      </c>
+      <c r="C80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B81" t="s">
+        <v>8</v>
+      </c>
+      <c r="C81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B82" t="s">
         <v>9</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B83" t="s">
+        <v>10</v>
+      </c>
+      <c r="C83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B84" t="s">
+        <v>11</v>
+      </c>
+      <c r="C84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B85" t="s">
+        <v>12</v>
+      </c>
+      <c r="C85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B86" t="s">
+        <v>13</v>
+      </c>
+      <c r="C86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B87" t="s">
+        <v>14</v>
+      </c>
+      <c r="C87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B88" t="s">
+        <v>15</v>
+      </c>
+      <c r="C88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B89" t="s">
+        <v>16</v>
+      </c>
+      <c r="C89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B90" t="s">
+        <v>17</v>
+      </c>
+      <c r="C90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B91" t="s">
+        <v>18</v>
+      </c>
+      <c r="C91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B92" t="s">
         <v>19</v>
+      </c>
+      <c r="C92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B93" t="s">
+        <v>20</v>
+      </c>
+      <c r="C93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B94" t="s">
+        <v>21</v>
+      </c>
+      <c r="C94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B95" t="s">
+        <v>22</v>
+      </c>
+      <c r="C95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B96" t="s">
+        <v>23</v>
+      </c>
+      <c r="C96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B97" t="s">
+        <v>24</v>
+      </c>
+      <c r="C97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B98" t="s">
+        <v>25</v>
+      </c>
+      <c r="C98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B99" t="s">
+        <v>26</v>
+      </c>
+      <c r="C99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B100" t="s">
+        <v>27</v>
+      </c>
+      <c r="C100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B101" t="s">
+        <v>28</v>
+      </c>
+      <c r="C101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B103" t="s">
+        <v>4</v>
+      </c>
+      <c r="C103">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B104" t="s">
+        <v>6</v>
+      </c>
+      <c r="C104">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B105" t="s">
+        <v>7</v>
+      </c>
+      <c r="C105">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B106" t="s">
+        <v>8</v>
+      </c>
+      <c r="C106">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B107" t="s">
+        <v>9</v>
+      </c>
+      <c r="C107">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B108" t="s">
+        <v>10</v>
+      </c>
+      <c r="C108">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B109" t="s">
+        <v>11</v>
+      </c>
+      <c r="C109">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B110" t="s">
+        <v>12</v>
+      </c>
+      <c r="C110">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B111" t="s">
+        <v>13</v>
+      </c>
+      <c r="C111">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B112" t="s">
+        <v>14</v>
+      </c>
+      <c r="C112">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B113" t="s">
+        <v>15</v>
+      </c>
+      <c r="C113">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B114" t="s">
+        <v>16</v>
+      </c>
+      <c r="C114">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B115" t="s">
+        <v>17</v>
+      </c>
+      <c r="C115">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B116" t="s">
+        <v>18</v>
+      </c>
+      <c r="C116">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B117" t="s">
+        <v>19</v>
+      </c>
+      <c r="C117">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B118" t="s">
+        <v>20</v>
+      </c>
+      <c r="C118">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B119" t="s">
+        <v>21</v>
+      </c>
+      <c r="C119">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B120" t="s">
+        <v>22</v>
+      </c>
+      <c r="C120">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B121" t="s">
+        <v>23</v>
+      </c>
+      <c r="C121">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B122" t="s">
+        <v>24</v>
+      </c>
+      <c r="C122">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B123" t="s">
+        <v>25</v>
+      </c>
+      <c r="C123">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B124" t="s">
+        <v>26</v>
+      </c>
+      <c r="C124">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B125" t="s">
+        <v>27</v>
+      </c>
+      <c r="C125">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B126" t="s">
+        <v>28</v>
+      </c>
+      <c r="C126">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B128" t="s">
+        <v>4</v>
+      </c>
+      <c r="C128">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B129" t="s">
+        <v>6</v>
+      </c>
+      <c r="C129">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B130" t="s">
+        <v>7</v>
+      </c>
+      <c r="C130">
+        <v>9.0675</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B131" t="s">
+        <v>8</v>
+      </c>
+      <c r="C131">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B132" t="s">
+        <v>9</v>
+      </c>
+      <c r="C132">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B133" t="s">
+        <v>10</v>
+      </c>
+      <c r="C133">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B134" t="s">
+        <v>11</v>
+      </c>
+      <c r="C134">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B135" t="s">
+        <v>12</v>
+      </c>
+      <c r="C135">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B136" t="s">
+        <v>13</v>
+      </c>
+      <c r="C136">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B137" t="s">
+        <v>14</v>
+      </c>
+      <c r="C137">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B138" t="s">
+        <v>15</v>
+      </c>
+      <c r="C138">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B139" t="s">
+        <v>16</v>
+      </c>
+      <c r="C139">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B140" t="s">
+        <v>17</v>
+      </c>
+      <c r="C140">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B141" t="s">
+        <v>18</v>
+      </c>
+      <c r="C141">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B142" t="s">
+        <v>19</v>
+      </c>
+      <c r="C142">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B143" t="s">
+        <v>20</v>
+      </c>
+      <c r="C143">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B144" t="s">
+        <v>21</v>
+      </c>
+      <c r="C144">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B145" t="s">
+        <v>22</v>
+      </c>
+      <c r="C145">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B146" t="s">
+        <v>23</v>
+      </c>
+      <c r="C146">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B147" t="s">
+        <v>24</v>
+      </c>
+      <c r="C147">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B148" t="s">
+        <v>25</v>
+      </c>
+      <c r="C148">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B149" t="s">
+        <v>26</v>
+      </c>
+      <c r="C149">
+        <v>9.0675</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B150" t="s">
+        <v>27</v>
+      </c>
+      <c r="C150">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B151" t="s">
+        <v>28</v>
+      </c>
+      <c r="C151">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B153" t="s">
+        <v>4</v>
+      </c>
+      <c r="C153">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B154" t="s">
+        <v>6</v>
+      </c>
+      <c r="C154">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B155" t="s">
+        <v>7</v>
+      </c>
+      <c r="C155">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B156" t="s">
+        <v>8</v>
+      </c>
+      <c r="C156">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B157" t="s">
+        <v>9</v>
+      </c>
+      <c r="C157">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B158" t="s">
+        <v>10</v>
+      </c>
+      <c r="C158">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B159" t="s">
+        <v>11</v>
+      </c>
+      <c r="C159">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B160" t="s">
+        <v>12</v>
+      </c>
+      <c r="C160">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B161" t="s">
+        <v>13</v>
+      </c>
+      <c r="C161">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B162" t="s">
+        <v>14</v>
+      </c>
+      <c r="C162">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B163" t="s">
+        <v>15</v>
+      </c>
+      <c r="C163">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B164" t="s">
+        <v>16</v>
+      </c>
+      <c r="C164">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B165" t="s">
+        <v>17</v>
+      </c>
+      <c r="C165">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B166" t="s">
+        <v>18</v>
+      </c>
+      <c r="C166">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B167" t="s">
+        <v>19</v>
+      </c>
+      <c r="C167">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B168" t="s">
+        <v>20</v>
+      </c>
+      <c r="C168">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B169" t="s">
+        <v>21</v>
+      </c>
+      <c r="C169">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B170" t="s">
+        <v>22</v>
+      </c>
+      <c r="C170">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A171" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B171" t="s">
+        <v>23</v>
+      </c>
+      <c r="C171">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B172" t="s">
+        <v>24</v>
+      </c>
+      <c r="C172">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A173" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B173" t="s">
+        <v>25</v>
+      </c>
+      <c r="C173">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A174" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B174" t="s">
+        <v>26</v>
+      </c>
+      <c r="C174">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A175" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B175" t="s">
+        <v>27</v>
+      </c>
+      <c r="C175">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B176" t="s">
+        <v>28</v>
+      </c>
+      <c r="C176">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A178" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B178" t="s">
+        <v>4</v>
+      </c>
+      <c r="C178">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A179" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B179" t="s">
+        <v>6</v>
+      </c>
+      <c r="C179">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A180" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B180" t="s">
+        <v>7</v>
+      </c>
+      <c r="C180">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A181" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B181" t="s">
+        <v>8</v>
+      </c>
+      <c r="C181">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A182" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B182" t="s">
+        <v>9</v>
+      </c>
+      <c r="C182">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A183" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B183" t="s">
+        <v>10</v>
+      </c>
+      <c r="C183">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A184" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B184" t="s">
+        <v>11</v>
+      </c>
+      <c r="C184">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A185" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B185" t="s">
+        <v>12</v>
+      </c>
+      <c r="C185">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A186" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B186" t="s">
+        <v>13</v>
+      </c>
+      <c r="C186">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A187" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B187" t="s">
+        <v>14</v>
+      </c>
+      <c r="C187">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A188" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B188" t="s">
+        <v>15</v>
+      </c>
+      <c r="C188">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A189" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B189" t="s">
+        <v>16</v>
+      </c>
+      <c r="C189">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A190" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B190" t="s">
+        <v>17</v>
+      </c>
+      <c r="C190">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A191" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B191" t="s">
+        <v>18</v>
+      </c>
+      <c r="C191">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A192" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B192" t="s">
+        <v>19</v>
+      </c>
+      <c r="C192">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A193" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B193" t="s">
+        <v>20</v>
+      </c>
+      <c r="C193">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A194" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B194" t="s">
+        <v>21</v>
+      </c>
+      <c r="C194">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A195" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B195" t="s">
+        <v>22</v>
+      </c>
+      <c r="C195">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A196" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B196" t="s">
+        <v>23</v>
+      </c>
+      <c r="C196">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A197" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B197" t="s">
+        <v>24</v>
+      </c>
+      <c r="C197">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A198" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B198" t="s">
+        <v>25</v>
+      </c>
+      <c r="C198">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A199" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B199" t="s">
+        <v>26</v>
+      </c>
+      <c r="C199">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A200" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B200" t="s">
+        <v>27</v>
+      </c>
+      <c r="C200">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A201" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B201" t="s">
+        <v>28</v>
+      </c>
+      <c r="C201">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A203" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B203" t="s">
+        <v>4</v>
+      </c>
+      <c r="C203">
+        <v>8833</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A204" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B204" t="s">
+        <v>6</v>
+      </c>
+      <c r="C204">
+        <v>8577</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A205" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B205" t="s">
+        <v>7</v>
+      </c>
+      <c r="C205">
+        <v>1921</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A206" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B206" t="s">
+        <v>8</v>
+      </c>
+      <c r="C206">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A207" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B207" t="s">
+        <v>9</v>
+      </c>
+      <c r="C207">
+        <v>8577</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A208" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B208" t="s">
+        <v>10</v>
+      </c>
+      <c r="C208">
+        <v>8321</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A209" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B209" t="s">
+        <v>11</v>
+      </c>
+      <c r="C209">
+        <v>8321</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A210" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B210" t="s">
+        <v>12</v>
+      </c>
+      <c r="C210">
+        <v>8577</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A211" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B211" t="s">
+        <v>13</v>
+      </c>
+      <c r="C211">
+        <v>8321</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A212" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B212" t="s">
+        <v>14</v>
+      </c>
+      <c r="C212">
+        <v>37504</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A213" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B213" t="s">
+        <v>15</v>
+      </c>
+      <c r="C213">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A214" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B214" t="s">
+        <v>16</v>
+      </c>
+      <c r="C214">
+        <v>57472</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A215" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B215" t="s">
+        <v>17</v>
+      </c>
+      <c r="C215">
+        <v>23168</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A216" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B216" t="s">
+        <v>18</v>
+      </c>
+      <c r="C216">
+        <v>8577</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A217" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B217" t="s">
+        <v>19</v>
+      </c>
+      <c r="C217">
+        <v>8577</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A218" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B218" t="s">
+        <v>20</v>
+      </c>
+      <c r="C218">
+        <v>8577</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A219" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B219" t="s">
+        <v>21</v>
+      </c>
+      <c r="C219">
+        <v>47744</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A220" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B220" t="s">
+        <v>22</v>
+      </c>
+      <c r="C220">
+        <v>62080</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A221" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B221" t="s">
+        <v>23</v>
+      </c>
+      <c r="C221">
+        <v>26496</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A222" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B222" t="s">
+        <v>24</v>
+      </c>
+      <c r="C222">
+        <v>20352</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A223" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B223" t="s">
+        <v>25</v>
+      </c>
+      <c r="C223">
+        <v>20096</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A224" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B224" t="s">
+        <v>26</v>
+      </c>
+      <c r="C224">
+        <v>23168</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A225" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B225" t="s">
+        <v>27</v>
+      </c>
+      <c r="C225">
+        <v>22656</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A226" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B226" t="s">
+        <v>28</v>
+      </c>
+      <c r="C226">
+        <v>10112</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A228" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B228" t="s">
+        <v>4</v>
+      </c>
+      <c r="C228" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A229" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B229" t="s">
+        <v>6</v>
+      </c>
+      <c r="C229" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A230" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B230" t="s">
+        <v>7</v>
+      </c>
+      <c r="C230" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A231" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B231" t="s">
+        <v>8</v>
+      </c>
+      <c r="C231" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A232" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B232" t="s">
+        <v>9</v>
+      </c>
+      <c r="C232" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A233" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B233" t="s">
+        <v>10</v>
+      </c>
+      <c r="C233" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A234" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B234" t="s">
+        <v>11</v>
+      </c>
+      <c r="C234" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A235" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B235" t="s">
+        <v>12</v>
+      </c>
+      <c r="C235" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A236" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B236" t="s">
+        <v>13</v>
+      </c>
+      <c r="C236" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A237" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B237" t="s">
+        <v>14</v>
+      </c>
+      <c r="C237" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A238" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B238" t="s">
+        <v>15</v>
+      </c>
+      <c r="C238" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A239" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B239" t="s">
+        <v>16</v>
+      </c>
+      <c r="C239" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A240" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B240" t="s">
+        <v>17</v>
+      </c>
+      <c r="C240" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A241" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B241" t="s">
+        <v>18</v>
+      </c>
+      <c r="C241" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A242" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B242" t="s">
+        <v>19</v>
+      </c>
+      <c r="C242" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A243" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B243" t="s">
+        <v>20</v>
+      </c>
+      <c r="C243" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A244" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B244" t="s">
+        <v>21</v>
+      </c>
+      <c r="C244" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A245" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B245" t="s">
+        <v>22</v>
+      </c>
+      <c r="C245" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A246" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B246" t="s">
+        <v>23</v>
+      </c>
+      <c r="C246" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A247" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B247" t="s">
+        <v>24</v>
+      </c>
+      <c r="C247" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A248" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B248" t="s">
+        <v>25</v>
+      </c>
+      <c r="C248" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A249" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B249" t="s">
+        <v>26</v>
+      </c>
+      <c r="C249" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A250" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B250" t="s">
+        <v>27</v>
+      </c>
+      <c r="C250" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A251" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B251" t="s">
+        <v>28</v>
+      </c>
+      <c r="C251" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
telegram bot without authentication
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="31">
   <si>
     <t>label</t>
   </si>
@@ -25,55 +25,85 @@
     <t>Об`єм (маса) каналу витрати 1</t>
   </si>
   <si>
-    <t>25:8:2020:1</t>
+    <t>9:9:2020:1</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>26:8:2020:1</t>
-  </si>
-  <si>
-    <t>27:8:2020:1</t>
-  </si>
-  <si>
-    <t>28:8:2020:1</t>
-  </si>
-  <si>
-    <t>29:8:2020:1</t>
-  </si>
-  <si>
-    <t>30:8:2020:1</t>
-  </si>
-  <si>
-    <t>1:9:2020:1</t>
-  </si>
-  <si>
-    <t>2:9:2020:1</t>
-  </si>
-  <si>
-    <t>3:9:2020:1</t>
-  </si>
-  <si>
-    <t>4:9:2020:1</t>
-  </si>
-  <si>
-    <t>5:9:2020:1</t>
-  </si>
-  <si>
-    <t>6:9:2020:1</t>
-  </si>
-  <si>
-    <t>7:9:2020:1</t>
-  </si>
-  <si>
-    <t>8:9:2020:1</t>
+    <t>10:9:2020:1</t>
+  </si>
+  <si>
+    <t>11:9:2020:1</t>
+  </si>
+  <si>
+    <t>12:9:2020:1</t>
+  </si>
+  <si>
+    <t>13:9:2020:1</t>
+  </si>
+  <si>
+    <t>14:9:2020:1</t>
+  </si>
+  <si>
+    <t>15:9:2020:1</t>
+  </si>
+  <si>
+    <t>16:9:2020:1</t>
+  </si>
+  <si>
+    <t>17:9:2020:1</t>
+  </si>
+  <si>
+    <t>18:9:2020:1</t>
+  </si>
+  <si>
+    <t>19:9:2020:1</t>
+  </si>
+  <si>
+    <t>20:9:2020:1</t>
+  </si>
+  <si>
+    <t>21:9:2020:1</t>
+  </si>
+  <si>
+    <t>22:9:2020:1</t>
+  </si>
+  <si>
+    <t>23:9:2020:1</t>
+  </si>
+  <si>
+    <t>24:9:2020:1</t>
+  </si>
+  <si>
+    <t>25:9:2020:1</t>
+  </si>
+  <si>
+    <t>26:9:2020:0</t>
+  </si>
+  <si>
+    <t>27:9:2020:0</t>
+  </si>
+  <si>
+    <t>28:9:2020:0</t>
+  </si>
+  <si>
+    <t>29:9:2020:0</t>
+  </si>
+  <si>
+    <t>30:9:2020:0</t>
+  </si>
+  <si>
+    <t>31:9:2020:0</t>
   </si>
   <si>
     <t>Значення температури ТСП 2 * 100</t>
   </si>
   <si>
     <t>Час роботи лічильника, год</t>
+  </si>
+  <si>
+    <t>Введені користувачем константи тиску * 1000</t>
   </si>
 </sst>
 </file>
@@ -454,7 +484,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C46"/>
+  <dimension ref="A1:C97"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="64" style="1" customWidth="1"/>
@@ -627,15 +657,26 @@
         <v>0</v>
       </c>
     </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+    </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C18">
-        <v>23.18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -643,10 +684,10 @@
         <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C19">
-        <v>23.47</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -654,10 +695,10 @@
         <v>5</v>
       </c>
       <c r="B20" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C20">
-        <v>23.48</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -665,10 +706,10 @@
         <v>5</v>
       </c>
       <c r="B21" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="C21">
-        <v>23.32</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -676,10 +717,10 @@
         <v>5</v>
       </c>
       <c r="B22" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="C22">
-        <v>23.43</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -687,10 +728,10 @@
         <v>5</v>
       </c>
       <c r="B23" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C23">
-        <v>23.47</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -698,10 +739,10 @@
         <v>5</v>
       </c>
       <c r="B24" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="C24">
-        <v>22.58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -709,32 +750,21 @@
         <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="C25">
-        <v>22.12</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B26" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26">
-        <v>22.03</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C27">
-        <v>23.55</v>
+        <v>22.72</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -742,10 +772,10 @@
         <v>5</v>
       </c>
       <c r="B28" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C28">
-        <v>22.72</v>
+        <v>21.8</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -753,10 +783,10 @@
         <v>5</v>
       </c>
       <c r="B29" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C29">
-        <v>22.34</v>
+        <v>22.18</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -764,10 +794,10 @@
         <v>5</v>
       </c>
       <c r="B30" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C30">
-        <v>22.74</v>
+        <v>22.8</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -775,21 +805,32 @@
         <v>5</v>
       </c>
       <c r="B31" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C31">
-        <v>22.95</v>
+        <v>22.85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32">
+        <v>-50</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="B33" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C33">
-        <v>9.13861111111111</v>
+        <v>-50</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -797,10 +838,10 @@
         <v>5</v>
       </c>
       <c r="B34" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C34">
-        <v>9.13861111111111</v>
+        <v>-50</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -808,10 +849,10 @@
         <v>5</v>
       </c>
       <c r="B35" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C35">
-        <v>9.13861111111111</v>
+        <v>-50</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -819,10 +860,10 @@
         <v>5</v>
       </c>
       <c r="B36" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C36">
-        <v>9.13861111111111</v>
+        <v>-50</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -830,10 +871,10 @@
         <v>5</v>
       </c>
       <c r="B37" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C37">
-        <v>9.13861111111111</v>
+        <v>-50</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -841,10 +882,10 @@
         <v>5</v>
       </c>
       <c r="B38" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C38">
-        <v>9.13861111111111</v>
+        <v>-50</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -852,10 +893,10 @@
         <v>5</v>
       </c>
       <c r="B39" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C39">
-        <v>9.13861111111111</v>
+        <v>-50</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -863,10 +904,10 @@
         <v>5</v>
       </c>
       <c r="B40" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C40">
-        <v>9.13861111111111</v>
+        <v>-50</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -874,10 +915,10 @@
         <v>5</v>
       </c>
       <c r="B41" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C41">
-        <v>9.13861111111111</v>
+        <v>-50</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -885,10 +926,10 @@
         <v>5</v>
       </c>
       <c r="B42" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C42">
-        <v>9.13861111111111</v>
+        <v>-50</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -896,10 +937,10 @@
         <v>5</v>
       </c>
       <c r="B43" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C43">
-        <v>9.13861111111111</v>
+        <v>-50</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -907,10 +948,10 @@
         <v>5</v>
       </c>
       <c r="B44" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C44">
-        <v>9.13861111111111</v>
+        <v>-50</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -918,10 +959,10 @@
         <v>5</v>
       </c>
       <c r="B45" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C45">
-        <v>9.13861111111111</v>
+        <v>-50</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -929,10 +970,549 @@
         <v>5</v>
       </c>
       <c r="B46" t="s">
+        <v>24</v>
+      </c>
+      <c r="C46">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B47" t="s">
+        <v>25</v>
+      </c>
+      <c r="C47">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B48" t="s">
+        <v>26</v>
+      </c>
+      <c r="C48">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B49" t="s">
+        <v>27</v>
+      </c>
+      <c r="C49">
+        <v>22.95</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B51" t="s">
+        <v>4</v>
+      </c>
+      <c r="C51">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B52" t="s">
+        <v>6</v>
+      </c>
+      <c r="C52">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B53" t="s">
+        <v>7</v>
+      </c>
+      <c r="C53">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B54" t="s">
+        <v>8</v>
+      </c>
+      <c r="C54">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B55" t="s">
+        <v>9</v>
+      </c>
+      <c r="C55">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B56" t="s">
+        <v>10</v>
+      </c>
+      <c r="C56">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B57" t="s">
+        <v>11</v>
+      </c>
+      <c r="C57">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B58" t="s">
+        <v>12</v>
+      </c>
+      <c r="C58">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B59" t="s">
+        <v>13</v>
+      </c>
+      <c r="C59">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B60" t="s">
+        <v>14</v>
+      </c>
+      <c r="C60">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B61" t="s">
+        <v>15</v>
+      </c>
+      <c r="C61">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B62" t="s">
+        <v>16</v>
+      </c>
+      <c r="C62">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B63" t="s">
+        <v>17</v>
+      </c>
+      <c r="C63">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B64" t="s">
         <v>18</v>
       </c>
-      <c r="C46">
-        <v>9.13861111111111</v>
+      <c r="C64">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B65" t="s">
+        <v>19</v>
+      </c>
+      <c r="C65">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B66" t="s">
+        <v>20</v>
+      </c>
+      <c r="C66">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B67" t="s">
+        <v>21</v>
+      </c>
+      <c r="C67">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B68" t="s">
+        <v>22</v>
+      </c>
+      <c r="C68">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B69" t="s">
+        <v>23</v>
+      </c>
+      <c r="C69">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B70" t="s">
+        <v>24</v>
+      </c>
+      <c r="C70">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B71" t="s">
+        <v>25</v>
+      </c>
+      <c r="C71">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B72" t="s">
+        <v>26</v>
+      </c>
+      <c r="C72">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B73" t="s">
+        <v>27</v>
+      </c>
+      <c r="C73">
+        <v>9.13861111111111</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B75" t="s">
+        <v>4</v>
+      </c>
+      <c r="C75">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B76" t="s">
+        <v>6</v>
+      </c>
+      <c r="C76">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B77" t="s">
+        <v>7</v>
+      </c>
+      <c r="C77">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B78" t="s">
+        <v>8</v>
+      </c>
+      <c r="C78">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B79" t="s">
+        <v>9</v>
+      </c>
+      <c r="C79">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B80" t="s">
+        <v>10</v>
+      </c>
+      <c r="C80">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B81" t="s">
+        <v>11</v>
+      </c>
+      <c r="C81">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B82" t="s">
+        <v>12</v>
+      </c>
+      <c r="C82">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B83" t="s">
+        <v>13</v>
+      </c>
+      <c r="C83">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B84" t="s">
+        <v>14</v>
+      </c>
+      <c r="C84">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B85" t="s">
+        <v>15</v>
+      </c>
+      <c r="C85">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B86" t="s">
+        <v>16</v>
+      </c>
+      <c r="C86">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B87" t="s">
+        <v>17</v>
+      </c>
+      <c r="C87">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B88" t="s">
+        <v>18</v>
+      </c>
+      <c r="C88">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B89" t="s">
+        <v>19</v>
+      </c>
+      <c r="C89">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B90" t="s">
+        <v>20</v>
+      </c>
+      <c r="C90">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B91" t="s">
+        <v>21</v>
+      </c>
+      <c r="C91">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B92" t="s">
+        <v>22</v>
+      </c>
+      <c r="C92">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B93" t="s">
+        <v>23</v>
+      </c>
+      <c r="C93">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B94" t="s">
+        <v>24</v>
+      </c>
+      <c r="C94">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B95" t="s">
+        <v>25</v>
+      </c>
+      <c r="C95">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B96" t="s">
+        <v>26</v>
+      </c>
+      <c r="C96">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B97" t="s">
+        <v>27</v>
+      </c>
+      <c r="C97">
+        <v>0.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
auth connect to server
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="39">
   <si>
     <t>label</t>
   </si>
@@ -25,24 +25,102 @@
     <t>Об`єм (маса) каналу витрати 1</t>
   </si>
   <si>
+    <t>12:9:2020:1</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>13:9:2020:1</t>
+  </si>
+  <si>
+    <t>14:9:2020:1</t>
+  </si>
+  <si>
+    <t>15:9:2020:1</t>
+  </si>
+  <si>
+    <t>16:9:2020:1</t>
+  </si>
+  <si>
+    <t>17:9:2020:1</t>
+  </si>
+  <si>
+    <t>18:9:2020:1</t>
+  </si>
+  <si>
+    <t>19:9:2020:1</t>
+  </si>
+  <si>
+    <t>20:9:2020:1</t>
+  </si>
+  <si>
+    <t>21:9:2020:1</t>
+  </si>
+  <si>
+    <t>22:9:2020:1</t>
+  </si>
+  <si>
+    <t>23:9:2020:1</t>
+  </si>
+  <si>
+    <t>24:9:2020:1</t>
+  </si>
+  <si>
+    <t>25:9:2020:1</t>
+  </si>
+  <si>
+    <t>26:9:2020:0</t>
+  </si>
+  <si>
+    <t>27:9:2020:0</t>
+  </si>
+  <si>
+    <t>28:9:2020:0</t>
+  </si>
+  <si>
+    <t>29:9:2020:0</t>
+  </si>
+  <si>
+    <t>30:9:2020:0</t>
+  </si>
+  <si>
+    <t>31:9:2020:0</t>
+  </si>
+  <si>
+    <t>1:10:2020:0</t>
+  </si>
+  <si>
+    <t>2:10:2020:0</t>
+  </si>
+  <si>
+    <t>3:10:2020:0</t>
+  </si>
+  <si>
+    <t>4:10:2020:0</t>
+  </si>
+  <si>
+    <t>5:10:2020:0</t>
+  </si>
+  <si>
+    <t>6:10:2020:0</t>
+  </si>
+  <si>
+    <t>7:10:2020:0</t>
+  </si>
+  <si>
+    <t>8:10:2020:0</t>
+  </si>
+  <si>
+    <t>9:10:2020:0</t>
+  </si>
+  <si>
     <t>10:10:2020:0</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>11:10:2020:0</t>
   </si>
   <si>
-    <t>12:10:2020:0</t>
-  </si>
-  <si>
-    <t>13:10:2020:0</t>
-  </si>
-  <si>
-    <t>14:10:2020:0</t>
-  </si>
-  <si>
     <t>Значення температури ТСП 1 * 100</t>
   </si>
   <si>
@@ -50,18 +128,6 @@
   </si>
   <si>
     <t>Тепло</t>
-  </si>
-  <si>
-    <t>Час роботи лічильника, год</t>
-  </si>
-  <si>
-    <t>Час помилок</t>
-  </si>
-  <si>
-    <t>Введені користувачем константи тиску * 1000</t>
-  </si>
-  <si>
-    <t>Спожита енергія</t>
   </si>
 </sst>
 </file>
@@ -442,7 +508,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C55"/>
+  <dimension ref="A1:C129"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="64" style="1" customWidth="1"/>
@@ -516,15 +582,26 @@
         <v>0</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+    </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C9">
-        <v>22.72</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -532,10 +609,10 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C10">
-        <v>22.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -543,10 +620,10 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C11">
-        <v>21.85</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -554,10 +631,10 @@
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C12">
-        <v>21.68</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -565,21 +642,32 @@
         <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C13">
-        <v>21.73</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C15">
-        <v>22.73</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -587,10 +675,10 @@
         <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C16">
-        <v>22.13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -598,10 +686,10 @@
         <v>5</v>
       </c>
       <c r="B17" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C17">
-        <v>21.84</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -609,10 +697,10 @@
         <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C18">
-        <v>21.73</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -620,18 +708,29 @@
         <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C19">
-        <v>21.77</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B21" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -642,7 +741,7 @@
         <v>5</v>
       </c>
       <c r="B22" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -653,7 +752,7 @@
         <v>5</v>
       </c>
       <c r="B23" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -664,7 +763,7 @@
         <v>5</v>
       </c>
       <c r="B24" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -675,21 +774,32 @@
         <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="C25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B27" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="C27">
-        <v>9.13861111111111</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -697,10 +807,10 @@
         <v>5</v>
       </c>
       <c r="B28" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="C28">
-        <v>9.13861111111111</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -708,10 +818,10 @@
         <v>5</v>
       </c>
       <c r="B29" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="C29">
-        <v>9.13861111111111</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -719,10 +829,10 @@
         <v>5</v>
       </c>
       <c r="B30" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="C30">
-        <v>9.13861111111111</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -730,43 +840,43 @@
         <v>5</v>
       </c>
       <c r="B31" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="C31">
-        <v>9.13861111111111</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B33" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="C33">
-        <v>9.13861111111111</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B34" t="s">
-        <v>6</v>
-      </c>
-      <c r="C34">
-        <v>9.13861111111111</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="B35" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C35">
-        <v>9.13861111111111</v>
+        <v>22.73</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -774,10 +884,10 @@
         <v>5</v>
       </c>
       <c r="B36" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C36">
-        <v>9.13861111111111</v>
+        <v>22.7</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -785,21 +895,32 @@
         <v>5</v>
       </c>
       <c r="B37" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C37">
-        <v>9.0675</v>
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B38" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38">
+        <v>-50</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B39" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C39">
-        <v>0.5</v>
+        <v>-50</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -807,10 +928,10 @@
         <v>5</v>
       </c>
       <c r="B40" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C40">
-        <v>0.5</v>
+        <v>-50</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -818,10 +939,10 @@
         <v>5</v>
       </c>
       <c r="B41" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C41">
-        <v>0.5</v>
+        <v>-50</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -829,10 +950,10 @@
         <v>5</v>
       </c>
       <c r="B42" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C42">
-        <v>0.5</v>
+        <v>-50</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -840,21 +961,32 @@
         <v>5</v>
       </c>
       <c r="B43" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C43">
-        <v>0.5</v>
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B44" t="s">
+        <v>14</v>
+      </c>
+      <c r="C44">
+        <v>-50</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B45" t="s">
         <v>15</v>
       </c>
-      <c r="B45" t="s">
-        <v>4</v>
-      </c>
       <c r="C45">
-        <v>0.4</v>
+        <v>-50</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -862,10 +994,10 @@
         <v>5</v>
       </c>
       <c r="B46" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C46">
-        <v>0.4</v>
+        <v>-50</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -873,10 +1005,10 @@
         <v>5</v>
       </c>
       <c r="B47" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C47">
-        <v>0.4</v>
+        <v>-50</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -884,10 +1016,10 @@
         <v>5</v>
       </c>
       <c r="B48" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C48">
-        <v>0.4</v>
+        <v>-50</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -895,21 +1027,32 @@
         <v>5</v>
       </c>
       <c r="B49" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C49">
-        <v>0.4</v>
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B50" t="s">
+        <v>20</v>
+      </c>
+      <c r="C50">
+        <v>-50</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B51" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C51">
-        <v>8833</v>
+        <v>-50</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -917,10 +1060,10 @@
         <v>5</v>
       </c>
       <c r="B52" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C52">
-        <v>8833</v>
+        <v>-50</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -928,10 +1071,10 @@
         <v>5</v>
       </c>
       <c r="B53" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C53">
-        <v>8833</v>
+        <v>-50</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -939,10 +1082,10 @@
         <v>5</v>
       </c>
       <c r="B54" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="C54">
-        <v>8577</v>
+        <v>22.97</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -950,10 +1093,802 @@
         <v>5</v>
       </c>
       <c r="B55" t="s">
+        <v>25</v>
+      </c>
+      <c r="C55">
+        <v>22.79</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B56" t="s">
+        <v>26</v>
+      </c>
+      <c r="C56">
+        <v>22.73</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B57" t="s">
+        <v>27</v>
+      </c>
+      <c r="C57">
+        <v>22.87</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B58" t="s">
+        <v>28</v>
+      </c>
+      <c r="C58">
+        <v>22.67</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B59" t="s">
+        <v>29</v>
+      </c>
+      <c r="C59">
+        <v>22.74</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B60" t="s">
+        <v>30</v>
+      </c>
+      <c r="C60">
+        <v>22.76</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B61" t="s">
+        <v>31</v>
+      </c>
+      <c r="C61">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B62" t="s">
+        <v>32</v>
+      </c>
+      <c r="C62">
+        <v>22.58</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B63" t="s">
+        <v>33</v>
+      </c>
+      <c r="C63">
+        <v>22.93</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B64" t="s">
+        <v>34</v>
+      </c>
+      <c r="C64">
+        <v>22.72</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B65" t="s">
+        <v>35</v>
+      </c>
+      <c r="C65">
+        <v>22.1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B67" t="s">
+        <v>4</v>
+      </c>
+      <c r="C67">
+        <v>22.8</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B68" t="s">
+        <v>6</v>
+      </c>
+      <c r="C68">
+        <v>22.85</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B69" t="s">
+        <v>7</v>
+      </c>
+      <c r="C69">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B70" t="s">
+        <v>8</v>
+      </c>
+      <c r="C70">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B71" t="s">
         <v>9</v>
       </c>
-      <c r="C55">
-        <v>1921</v>
+      <c r="C71">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B72" t="s">
+        <v>10</v>
+      </c>
+      <c r="C72">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B73" t="s">
+        <v>11</v>
+      </c>
+      <c r="C73">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B74" t="s">
+        <v>12</v>
+      </c>
+      <c r="C74">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B75" t="s">
+        <v>13</v>
+      </c>
+      <c r="C75">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B76" t="s">
+        <v>14</v>
+      </c>
+      <c r="C76">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B77" t="s">
+        <v>15</v>
+      </c>
+      <c r="C77">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B78" t="s">
+        <v>16</v>
+      </c>
+      <c r="C78">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B79" t="s">
+        <v>17</v>
+      </c>
+      <c r="C79">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B80" t="s">
+        <v>18</v>
+      </c>
+      <c r="C80">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B81" t="s">
+        <v>19</v>
+      </c>
+      <c r="C81">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B82" t="s">
+        <v>20</v>
+      </c>
+      <c r="C82">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B83" t="s">
+        <v>21</v>
+      </c>
+      <c r="C83">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B84" t="s">
+        <v>22</v>
+      </c>
+      <c r="C84">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B85" t="s">
+        <v>23</v>
+      </c>
+      <c r="C85">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B86" t="s">
+        <v>24</v>
+      </c>
+      <c r="C86">
+        <v>22.95</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B87" t="s">
+        <v>25</v>
+      </c>
+      <c r="C87">
+        <v>22.73</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B88" t="s">
+        <v>26</v>
+      </c>
+      <c r="C88">
+        <v>22.7</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B89" t="s">
+        <v>27</v>
+      </c>
+      <c r="C89">
+        <v>22.89</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B90" t="s">
+        <v>28</v>
+      </c>
+      <c r="C90">
+        <v>22.71</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B91" t="s">
+        <v>29</v>
+      </c>
+      <c r="C91">
+        <v>22.75</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B92" t="s">
+        <v>30</v>
+      </c>
+      <c r="C92">
+        <v>22.8</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B93" t="s">
+        <v>31</v>
+      </c>
+      <c r="C93">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B94" t="s">
+        <v>32</v>
+      </c>
+      <c r="C94">
+        <v>22.54</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B95" t="s">
+        <v>33</v>
+      </c>
+      <c r="C95">
+        <v>22.93</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B96" t="s">
+        <v>34</v>
+      </c>
+      <c r="C96">
+        <v>22.73</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B97" t="s">
+        <v>35</v>
+      </c>
+      <c r="C97">
+        <v>22.13</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B99" t="s">
+        <v>4</v>
+      </c>
+      <c r="C99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B100" t="s">
+        <v>6</v>
+      </c>
+      <c r="C100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B101" t="s">
+        <v>7</v>
+      </c>
+      <c r="C101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B102" t="s">
+        <v>8</v>
+      </c>
+      <c r="C102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B103" t="s">
+        <v>9</v>
+      </c>
+      <c r="C103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B104" t="s">
+        <v>10</v>
+      </c>
+      <c r="C104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B105" t="s">
+        <v>11</v>
+      </c>
+      <c r="C105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B106" t="s">
+        <v>12</v>
+      </c>
+      <c r="C106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B107" t="s">
+        <v>13</v>
+      </c>
+      <c r="C107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B108" t="s">
+        <v>14</v>
+      </c>
+      <c r="C108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B109" t="s">
+        <v>15</v>
+      </c>
+      <c r="C109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B110" t="s">
+        <v>16</v>
+      </c>
+      <c r="C110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B111" t="s">
+        <v>17</v>
+      </c>
+      <c r="C111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B112" t="s">
+        <v>18</v>
+      </c>
+      <c r="C112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B113" t="s">
+        <v>19</v>
+      </c>
+      <c r="C113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B114" t="s">
+        <v>20</v>
+      </c>
+      <c r="C114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B115" t="s">
+        <v>21</v>
+      </c>
+      <c r="C115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B116" t="s">
+        <v>22</v>
+      </c>
+      <c r="C116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B117" t="s">
+        <v>23</v>
+      </c>
+      <c r="C117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B118" t="s">
+        <v>24</v>
+      </c>
+      <c r="C118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B119" t="s">
+        <v>25</v>
+      </c>
+      <c r="C119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B120" t="s">
+        <v>26</v>
+      </c>
+      <c r="C120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B121" t="s">
+        <v>27</v>
+      </c>
+      <c r="C121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B122" t="s">
+        <v>28</v>
+      </c>
+      <c r="C122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B123" t="s">
+        <v>29</v>
+      </c>
+      <c r="C123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B124" t="s">
+        <v>30</v>
+      </c>
+      <c r="C124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B125" t="s">
+        <v>31</v>
+      </c>
+      <c r="C125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B126" t="s">
+        <v>32</v>
+      </c>
+      <c r="C126">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B127" t="s">
+        <v>33</v>
+      </c>
+      <c r="C127">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B128" t="s">
+        <v>34</v>
+      </c>
+      <c r="C128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B129" t="s">
+        <v>35</v>
+      </c>
+      <c r="C129">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>